<commit_message>
Created a function for importing previous month's input tax.
</commit_message>
<xml_diff>
--- a/Main_Sheet.xlsx
+++ b/Main_Sheet.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
-    <t xml:space="preserve">Kod_urzedu</t>
+    <t xml:space="preserve">KodUrzedu</t>
   </si>
   <si>
     <t xml:space="preserve">Miesiac</t>
@@ -36,13 +36,13 @@
     <t xml:space="preserve">NIP</t>
   </si>
   <si>
-    <t xml:space="preserve">Nazwa</t>
+    <t xml:space="preserve">PelnaNazwa</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Nr_tel</t>
+    <t xml:space="preserve">Telefon</t>
   </si>
   <si>
     <t xml:space="preserve">Nucysfera</t>
@@ -667,10 +667,10 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
@@ -758,9 +758,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.28"/>
@@ -848,7 +848,7 @@
       <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>

</xml_diff>

<commit_message>
Sales export and import implemented.
</commit_message>
<xml_diff>
--- a/Main_Sheet.xlsx
+++ b/Main_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Witaj" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t xml:space="preserve">KodUrzedu</t>
   </si>
@@ -60,10 +60,37 @@
     <t xml:space="preserve">Kraj</t>
   </si>
   <si>
-    <t xml:space="preserve">NIP nabywcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nazwa nabywcy</t>
+    <t xml:space="preserve">NIP_nabywcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazwa_nabywcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nr_faktury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data_faktury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwota_netto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwota_podatku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PETRA-TRANS LOGISTYKA INWESTYCJE PIOTR WÓJCIAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faktura VAT 01/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIP sprzedawcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazwa sprzedawcy</t>
   </si>
   <si>
     <t xml:space="preserve">Nr faktury</t>
@@ -76,21 +103,6 @@
   </si>
   <si>
     <t xml:space="preserve">Kwota podatku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PETRA-TRANS LOGISTYKA INWESTYCJE PIOTR WÓJCIAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faktura VAT 01/03/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIP sprzedawcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nazwa sprzedawcy</t>
   </si>
   <si>
     <t xml:space="preserve">STANET S.C.</t>
@@ -462,12 +474,12 @@
   <autoFilter ref="B1:H2"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Kraj"/>
-    <tableColumn id="2" name="NIP nabywcy"/>
-    <tableColumn id="3" name="Nazwa nabywcy"/>
-    <tableColumn id="4" name="Nr faktury"/>
-    <tableColumn id="5" name="Data faktury"/>
-    <tableColumn id="6" name="Kwota netto"/>
-    <tableColumn id="7" name="Kwota podatku"/>
+    <tableColumn id="2" name="NIP_nabywcy"/>
+    <tableColumn id="3" name="Nazwa_nabywcy"/>
+    <tableColumn id="4" name="Nr_faktury"/>
+    <tableColumn id="5" name="Data_faktury"/>
+    <tableColumn id="6" name="Kwota_netto"/>
+    <tableColumn id="7" name="Kwota_podatku"/>
   </tableColumns>
 </table>
 </file>
@@ -666,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -754,8 +766,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -818,6 +830,32 @@
         <v>330000</v>
       </c>
       <c r="H2" s="14" t="n">
+        <v>75900</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>735103039</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>45747</v>
+      </c>
+      <c r="G3" s="13" t="n">
+        <v>330000</v>
+      </c>
+      <c r="H3" s="14" t="n">
         <v>75900</v>
       </c>
     </row>
@@ -871,16 +909,16 @@
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -894,10 +932,10 @@
         <v>6762646904</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F2" s="16" t="n">
         <v>45721</v>
@@ -920,10 +958,10 @@
         <v>5260250995</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F3" s="20" t="n">
         <v>45722</v>

</xml_diff>

<commit_message>
Generated file is accepted by jpk web.
</commit_message>
<xml_diff>
--- a/Main_Sheet.xlsx
+++ b/Main_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Witaj" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t xml:space="preserve">KodUrzedu</t>
   </si>
@@ -87,22 +87,10 @@
     <t xml:space="preserve">Faktura VAT 01/03/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">NIP sprzedawcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nazwa sprzedawcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nr faktury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data faktury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kwota netto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kwota podatku</t>
+    <t xml:space="preserve">NIP_sprzedawcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazwa_sprzedawcy</t>
   </si>
   <si>
     <t xml:space="preserve">STANET S.C.</t>
@@ -489,12 +477,12 @@
   <autoFilter ref="B1:H3"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Kraj"/>
-    <tableColumn id="2" name="NIP sprzedawcy"/>
-    <tableColumn id="3" name="Nazwa sprzedawcy"/>
-    <tableColumn id="4" name="Nr faktury"/>
-    <tableColumn id="5" name="Data faktury"/>
-    <tableColumn id="6" name="Kwota netto"/>
-    <tableColumn id="7" name="Kwota podatku"/>
+    <tableColumn id="2" name="NIP_sprzedawcy"/>
+    <tableColumn id="3" name="Nazwa_sprzedawcy"/>
+    <tableColumn id="4" name="Nr_faktury"/>
+    <tableColumn id="5" name="Data_faktury"/>
+    <tableColumn id="6" name="Kwota_netto"/>
+    <tableColumn id="7" name="Kwota_podatku"/>
   </tableColumns>
 </table>
 </file>
@@ -766,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -835,7 +823,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>18</v>
@@ -882,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -909,16 +897,16 @@
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -932,10 +920,10 @@
         <v>6762646904</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="16" t="n">
         <v>45721</v>
@@ -958,10 +946,10 @@
         <v>5260250995</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="20" t="n">
         <v>45722</v>

</xml_diff>